<commit_message>
create script tc_214, selection unit period two option show,
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/boatAndCarParking.xlsx
+++ b/src/test/resources/testdata/boatAndCarParking.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talhatahir\git\Marina\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha.tahir\git\Marina\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48386152-B9D4-434E-8E89-E50079EBB313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15165" windowHeight="6405"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginData" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>NAME</t>
   </si>
@@ -84,12 +85,15 @@
   </si>
   <si>
     <t>$/period</t>
+  </si>
+  <si>
+    <t>$/ft/period</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -126,10 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,11 +412,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,10 +436,10 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -456,11 +459,11 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>19</v>
+      <c r="D2" t="s">
+        <v>20</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -479,17 +482,17 @@
       <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -502,69 +505,69 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
+      <c r="D4" t="s">
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="C5"/>
+      <c r="D5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6"/>
+      <c r="D6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="C7"/>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8"/>
+      <c r="D8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9"/>
+      <c r="D9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10"/>
+      <c r="D10"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11"/>
+      <c r="D11"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12"/>
+      <c r="D12"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13"/>
+      <c r="D13"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="C14"/>
+      <c r="D14"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15"/>
+      <c r="D15"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" display="REDHATredhat1!@#"/>
+    <hyperlink ref="B4" r:id="rId1" display="REDHATredhat1!@#" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>

</xml_diff>